<commit_message>
Updated to version accepted in Marine Ecology
</commit_message>
<xml_diff>
--- a/fecal_data_final.xlsx
+++ b/fecal_data_final.xlsx
@@ -1,211 +1,218 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://niva365-my.sharepoint.com/personal/kristina_kvile_niva_no/Documents/SeedMoney-KVI-2021/CopeLinkExp2021/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_873E0DE786E1BB4B576384CC1619AED9694B43BC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
-  <si>
-    <t xml:space="preserve">DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXPERIMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHEEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOTTLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TREATMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TUBE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PELLETS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DURATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INT_CONC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXP_FIG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SACLA-FE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETHANOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also image 34-35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHYTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SACLA-FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bottle B only 2 pellets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Bottle B maybe 1 pellet)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAMHY-FE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAMHY-FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Many more pellets in total, &gt;&gt;100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lost by accident</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUICK-EXTRACT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A lot of pellets, &gt;&gt;200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A lot of algae material in the water, but only one pellet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also a lot of detritus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A lot of pellets, &gt;100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A couple got lost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Picture of algae material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Picture of rhodomonas pellet for comparison. A lot more pellets available.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="62">
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>EXPERIMENT</t>
+  </si>
+  <si>
+    <t>WHEEL</t>
+  </si>
+  <si>
+    <t>BOTTLE</t>
+  </si>
+  <si>
+    <t>TREATMENT</t>
+  </si>
+  <si>
+    <t>IMG</t>
+  </si>
+  <si>
+    <t>MAG</t>
+  </si>
+  <si>
+    <t>PRES</t>
+  </si>
+  <si>
+    <t>TUBE</t>
+  </si>
+  <si>
+    <t>PELLETS</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>DURATION</t>
+  </si>
+  <si>
+    <t>INT_CONC</t>
+  </si>
+  <si>
+    <t>EXP_FIG</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>SACLA-FE</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>ETHANOL</t>
+  </si>
+  <si>
+    <t>Also image 34-35</t>
+  </si>
+  <si>
+    <t>24h</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>PHYTO</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>SACLA-FR</t>
+  </si>
+  <si>
+    <t>Bottle B only 2 pellets</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>(Bottle B maybe 1 pellet)</t>
+  </si>
+  <si>
+    <t>LAMHY-FE</t>
+  </si>
+  <si>
+    <t>LAMHY-FR</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>Many more pellets in total, &gt;&gt;100</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Lost by accident</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>QUICK-EXTRACT</t>
+  </si>
+  <si>
+    <t>A lot of pellets, &gt;&gt;200</t>
+  </si>
+  <si>
+    <t>50?</t>
+  </si>
+  <si>
+    <t>A lot of algae material in the water, but only one pellet</t>
+  </si>
+  <si>
+    <t>Also a lot of detritus</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>A lot of pellets, &gt;100</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>A couple got lost</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>5B</t>
+  </si>
+  <si>
+    <t>48h</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Picture of algae material</t>
+  </si>
+  <si>
+    <t>Picture of rhodomonas pellet for comparison. A lot more pellets available.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -241,12 +248,21 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -528,14 +544,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -579,14 +597,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1">
         <v>44364</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -595,7 +613,7 @@
       <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>33</v>
       </c>
       <c r="G2" t="s">
@@ -604,10 +622,9 @@
       <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>30</v>
       </c>
-      <c r="J2"/>
       <c r="K2" t="s">
         <v>19</v>
       </c>
@@ -621,14 +638,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1">
         <v>44364</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
@@ -637,7 +654,7 @@
       <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>36</v>
       </c>
       <c r="G3" t="s">
@@ -646,11 +663,9 @@
       <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3">
         <v>31</v>
       </c>
-      <c r="J3"/>
-      <c r="K3"/>
       <c r="L3" t="s">
         <v>20</v>
       </c>
@@ -661,14 +676,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1">
         <v>44365</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
@@ -677,7 +692,7 @@
       <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>68</v>
       </c>
       <c r="G4" t="s">
@@ -686,13 +701,12 @@
       <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4">
         <v>42</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4">
         <v>19</v>
       </c>
-      <c r="K4"/>
       <c r="L4" t="s">
         <v>20</v>
       </c>
@@ -703,14 +717,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1">
         <v>44365</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
@@ -719,7 +733,7 @@
       <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>69</v>
       </c>
       <c r="G5" t="s">
@@ -728,10 +742,10 @@
       <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5">
         <v>43</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J5">
         <v>3</v>
       </c>
       <c r="K5" t="s">
@@ -747,14 +761,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1">
         <v>44365</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
@@ -763,7 +777,7 @@
       <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>70</v>
       </c>
       <c r="G6" t="s">
@@ -772,10 +786,10 @@
       <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6">
         <v>44</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6">
         <v>41</v>
       </c>
       <c r="K6" t="s">
@@ -791,14 +805,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1">
         <v>44365</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
@@ -807,18 +821,15 @@
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7"/>
-      <c r="G7"/>
       <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7">
         <v>45</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="K7"/>
       <c r="L7" t="s">
         <v>20</v>
       </c>
@@ -829,14 +840,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1">
         <v>44365</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
@@ -845,7 +856,7 @@
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>71</v>
       </c>
       <c r="G8" t="s">
@@ -854,13 +865,12 @@
       <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8">
         <v>45</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8">
         <v>3</v>
       </c>
-      <c r="K8"/>
       <c r="L8" t="s">
         <v>20</v>
       </c>
@@ -871,14 +881,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1">
         <v>44365</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
@@ -887,7 +897,7 @@
       <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>72</v>
       </c>
       <c r="G9" t="s">
@@ -896,11 +906,9 @@
       <c r="H9" t="s">
         <v>18</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9">
         <v>46</v>
       </c>
-      <c r="J9"/>
-      <c r="K9"/>
       <c r="L9" t="s">
         <v>20</v>
       </c>
@@ -911,14 +919,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1">
         <v>44365</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
@@ -927,18 +935,15 @@
       <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="F10"/>
-      <c r="G10"/>
       <c r="H10" t="s">
         <v>18</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10">
         <v>46</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J10">
         <v>4</v>
       </c>
-      <c r="K10"/>
       <c r="L10" t="s">
         <v>20</v>
       </c>
@@ -949,14 +954,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1">
         <v>44369</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
@@ -965,7 +970,7 @@
       <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>110</v>
       </c>
       <c r="G11" t="s">
@@ -974,10 +979,10 @@
       <c r="H11" t="s">
         <v>38</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11">
         <v>23</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J11">
         <v>40</v>
       </c>
       <c r="K11" t="s">
@@ -993,14 +998,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1">
         <v>44369</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
@@ -1009,7 +1014,7 @@
       <c r="E12" t="s">
         <v>16</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>113</v>
       </c>
       <c r="G12" t="s">
@@ -1018,13 +1023,12 @@
       <c r="H12" t="s">
         <v>38</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12">
         <v>25</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J12">
         <v>17</v>
       </c>
-      <c r="K12"/>
       <c r="L12" t="s">
         <v>20</v>
       </c>
@@ -1035,14 +1039,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1">
         <v>44369</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
@@ -1051,7 +1055,7 @@
       <c r="E13" t="s">
         <v>16</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>114</v>
       </c>
       <c r="G13" t="s">
@@ -1060,13 +1064,12 @@
       <c r="H13" t="s">
         <v>38</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13">
         <v>26</v>
       </c>
-      <c r="J13" t="n">
+      <c r="J13">
         <v>5</v>
       </c>
-      <c r="K13"/>
       <c r="L13" t="s">
         <v>20</v>
       </c>
@@ -1077,14 +1080,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1">
         <v>44369</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
@@ -1093,7 +1096,7 @@
       <c r="E14" t="s">
         <v>40</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>115</v>
       </c>
       <c r="G14" t="s">
@@ -1102,13 +1105,12 @@
       <c r="H14" t="s">
         <v>38</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14">
         <v>27</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J14">
         <v>11</v>
       </c>
-      <c r="K14"/>
       <c r="L14" t="s">
         <v>20</v>
       </c>
@@ -1119,14 +1121,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1">
         <v>44370</v>
       </c>
       <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
@@ -1135,11 +1137,6 @@
       <c r="E15" t="s">
         <v>34</v>
       </c>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
       <c r="K15" t="s">
         <v>42</v>
       </c>
@@ -1153,14 +1150,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1">
         <v>44370</v>
       </c>
       <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
@@ -1169,11 +1166,6 @@
       <c r="E16" t="s">
         <v>40</v>
       </c>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
       <c r="K16" t="s">
         <v>43</v>
       </c>
@@ -1187,14 +1179,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1">
         <v>44370</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
@@ -1203,7 +1195,7 @@
       <c r="E17" t="s">
         <v>34</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>153</v>
       </c>
       <c r="G17" t="s">
@@ -1212,13 +1204,12 @@
       <c r="H17" t="s">
         <v>45</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I17">
         <v>37</v>
       </c>
-      <c r="J17" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17"/>
+      <c r="J17">
+        <v>1</v>
+      </c>
       <c r="L17" t="s">
         <v>20</v>
       </c>
@@ -1229,14 +1220,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1">
         <v>44370</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
@@ -1245,7 +1236,7 @@
       <c r="E18" t="s">
         <v>24</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>154</v>
       </c>
       <c r="G18" t="s">
@@ -1254,10 +1245,10 @@
       <c r="H18" t="s">
         <v>45</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18">
         <v>38</v>
       </c>
-      <c r="J18" t="n">
+      <c r="J18">
         <v>45</v>
       </c>
       <c r="K18" t="s">
@@ -1273,14 +1264,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1">
         <v>44370</v>
       </c>
       <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
@@ -1289,7 +1280,7 @@
       <c r="E19" t="s">
         <v>35</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>155</v>
       </c>
       <c r="G19" t="s">
@@ -1298,10 +1289,10 @@
       <c r="H19" t="s">
         <v>45</v>
       </c>
-      <c r="I19" t="n">
+      <c r="I19">
         <v>39</v>
       </c>
-      <c r="J19" t="n">
+      <c r="J19">
         <v>1</v>
       </c>
       <c r="K19" t="s">
@@ -1317,14 +1308,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1">
         <v>44370</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
@@ -1333,7 +1324,7 @@
       <c r="E20" t="s">
         <v>35</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>156</v>
       </c>
       <c r="G20" t="s">
@@ -1342,10 +1333,10 @@
       <c r="H20" t="s">
         <v>45</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20">
         <v>39</v>
       </c>
-      <c r="J20" t="n">
+      <c r="J20">
         <v>3</v>
       </c>
       <c r="K20" t="s">
@@ -1361,14 +1352,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1">
         <v>44371</v>
       </c>
       <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
@@ -1377,18 +1368,15 @@
       <c r="E21" t="s">
         <v>40</v>
       </c>
-      <c r="F21"/>
-      <c r="G21"/>
       <c r="H21" t="s">
         <v>18</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I21">
         <v>70</v>
       </c>
-      <c r="J21" t="n">
+      <c r="J21">
         <v>3</v>
       </c>
-      <c r="K21"/>
       <c r="L21" t="s">
         <v>20</v>
       </c>
@@ -1399,14 +1387,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1">
         <v>44371</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
@@ -1415,18 +1403,15 @@
       <c r="E22" t="s">
         <v>16</v>
       </c>
-      <c r="F22"/>
-      <c r="G22"/>
       <c r="H22" t="s">
         <v>18</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I22">
         <v>71</v>
       </c>
-      <c r="J22" t="n">
+      <c r="J22">
         <v>4</v>
       </c>
-      <c r="K22"/>
       <c r="L22" t="s">
         <v>20</v>
       </c>
@@ -1437,14 +1422,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1">
         <v>44371</v>
       </c>
       <c r="B23" t="s">
         <v>50</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
@@ -1453,7 +1438,7 @@
       <c r="E23" t="s">
         <v>28</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>157</v>
       </c>
       <c r="G23" t="s">
@@ -1462,13 +1447,12 @@
       <c r="H23" t="s">
         <v>18</v>
       </c>
-      <c r="I23" t="n">
+      <c r="I23">
         <v>72</v>
       </c>
-      <c r="J23" t="n">
+      <c r="J23">
         <v>5</v>
       </c>
-      <c r="K23"/>
       <c r="L23" t="s">
         <v>20</v>
       </c>
@@ -1479,14 +1463,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1">
         <v>44371</v>
       </c>
       <c r="B24" t="s">
         <v>50</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
@@ -1495,7 +1479,7 @@
       <c r="E24" t="s">
         <v>16</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24">
         <v>158</v>
       </c>
       <c r="G24" t="s">
@@ -1504,13 +1488,12 @@
       <c r="H24" t="s">
         <v>18</v>
       </c>
-      <c r="I24" t="n">
+      <c r="I24">
         <v>73</v>
       </c>
-      <c r="J24" t="n">
+      <c r="J24">
         <v>8</v>
       </c>
-      <c r="K24"/>
       <c r="L24" t="s">
         <v>20</v>
       </c>
@@ -1521,14 +1504,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1">
         <v>44371</v>
       </c>
       <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
@@ -1537,17 +1520,16 @@
       <c r="E25" t="s">
         <v>24</v>
       </c>
-      <c r="F25"/>
       <c r="G25" t="s">
         <v>52</v>
       </c>
       <c r="H25" t="s">
         <v>18</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I25">
         <v>74</v>
       </c>
-      <c r="J25" t="n">
+      <c r="J25">
         <v>42</v>
       </c>
       <c r="K25" t="s">
@@ -1563,14 +1545,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="1">
         <v>44371</v>
       </c>
       <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
@@ -1579,7 +1561,7 @@
       <c r="E26" t="s">
         <v>34</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26">
         <v>161</v>
       </c>
       <c r="G26" t="s">
@@ -1588,10 +1570,10 @@
       <c r="H26" t="s">
         <v>18</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I26">
         <v>76</v>
       </c>
-      <c r="J26" t="n">
+      <c r="J26">
         <v>3</v>
       </c>
       <c r="K26" t="s">
@@ -1607,14 +1589,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1">
         <v>44371</v>
       </c>
       <c r="B27" t="s">
         <v>50</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
@@ -1623,18 +1605,15 @@
       <c r="E27" t="s">
         <v>35</v>
       </c>
-      <c r="F27"/>
-      <c r="G27"/>
       <c r="H27" t="s">
         <v>18</v>
       </c>
-      <c r="I27" t="n">
+      <c r="I27">
         <v>78</v>
       </c>
-      <c r="J27" t="n">
+      <c r="J27">
         <v>3</v>
       </c>
-      <c r="K27"/>
       <c r="L27" t="s">
         <v>20</v>
       </c>
@@ -1645,14 +1624,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1">
         <v>44372</v>
       </c>
       <c r="B28" t="s">
         <v>57</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
@@ -1661,14 +1640,9 @@
       <c r="E28" t="s">
         <v>40</v>
       </c>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-      <c r="J28" t="n">
+      <c r="J28">
         <v>0</v>
       </c>
-      <c r="K28"/>
       <c r="L28" t="s">
         <v>58</v>
       </c>
@@ -1679,14 +1653,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="1">
         <v>44372</v>
       </c>
       <c r="B29" t="s">
         <v>57</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
@@ -1695,14 +1669,9 @@
       <c r="E29" t="s">
         <v>16</v>
       </c>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-      <c r="J29" t="n">
+      <c r="J29">
         <v>0</v>
       </c>
-      <c r="K29"/>
       <c r="L29" t="s">
         <v>58</v>
       </c>
@@ -1713,14 +1682,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1">
         <v>44372</v>
       </c>
       <c r="B30" t="s">
         <v>57</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
@@ -1729,14 +1698,9 @@
       <c r="E30" t="s">
         <v>28</v>
       </c>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
-      <c r="J30" t="n">
+      <c r="J30">
         <v>0</v>
       </c>
-      <c r="K30"/>
       <c r="L30" t="s">
         <v>58</v>
       </c>
@@ -1747,14 +1711,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1">
         <v>44372</v>
       </c>
       <c r="B31" t="s">
         <v>57</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
@@ -1763,15 +1727,13 @@
       <c r="E31" t="s">
         <v>16</v>
       </c>
-      <c r="F31" t="n">
+      <c r="F31">
         <v>200</v>
       </c>
       <c r="G31" t="s">
         <v>59</v>
       </c>
-      <c r="H31"/>
-      <c r="I31"/>
-      <c r="J31" t="n">
+      <c r="J31">
         <v>0</v>
       </c>
       <c r="K31" t="s">
@@ -1787,14 +1749,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1">
         <v>44372</v>
       </c>
       <c r="B32" t="s">
         <v>57</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
@@ -1803,7 +1765,7 @@
       <c r="E32" t="s">
         <v>24</v>
       </c>
-      <c r="F32" t="n">
+      <c r="F32">
         <v>203</v>
       </c>
       <c r="G32" t="s">
@@ -1812,10 +1774,10 @@
       <c r="H32" t="s">
         <v>18</v>
       </c>
-      <c r="I32" t="n">
+      <c r="I32">
         <v>92</v>
       </c>
-      <c r="J32" t="n">
+      <c r="J32">
         <v>30</v>
       </c>
       <c r="K32" t="s">
@@ -1833,6 +1795,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>